<commit_message>
Changed title of plane wave lab
</commit_message>
<xml_diff>
--- a/StudentGuideModule2/what_labs_to_include/132 lab list for 2018fall.xlsx
+++ b/StudentGuideModule2/what_labs_to_include/132 lab list for 2018fall.xlsx
@@ -1305,9 +1305,6 @@
     <t>Deriving Electromagnetic Waves</t>
   </si>
   <si>
-    <t>Electromagnetic Plane Waves</t>
-  </si>
-  <si>
     <t>The Diffraction Grating</t>
   </si>
   <si>
@@ -1566,6 +1563,9 @@
   </si>
   <si>
     <t>Waves in Media, and Deriving Snell's Law</t>
+  </si>
+  <si>
+    <t>Visualizing Electromagnetic Plane Waves</t>
   </si>
 </sst>
 </file>
@@ -2795,8 +2795,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T48" sqref="T48"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2827,7 +2828,7 @@
         <v>107</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D1" s="50" t="s">
         <v>85</v>
@@ -2836,19 +2837,19 @@
         <v>86</v>
       </c>
       <c r="F1" s="50" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G1" s="50" t="s">
+        <v>179</v>
+      </c>
+      <c r="H1" s="50" t="s">
         <v>180</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="I1" s="50" t="s">
         <v>181</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="J1" s="50" t="s">
         <v>182</v>
-      </c>
-      <c r="J1" s="50" t="s">
-        <v>183</v>
       </c>
       <c r="K1" s="51" t="s">
         <v>108</v>
@@ -2857,22 +2858,22 @@
         <v>109</v>
       </c>
       <c r="M1" s="49" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N1" s="49" t="s">
         <v>100</v>
       </c>
       <c r="O1" s="49" t="s">
+        <v>201</v>
+      </c>
+      <c r="P1" s="49" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q1" s="49" t="s">
+        <v>199</v>
+      </c>
+      <c r="R1" s="52" t="s">
         <v>202</v>
-      </c>
-      <c r="P1" s="49" t="s">
-        <v>201</v>
-      </c>
-      <c r="Q1" s="49" t="s">
-        <v>200</v>
-      </c>
-      <c r="R1" s="52" t="s">
-        <v>203</v>
       </c>
       <c r="S1" s="32"/>
       <c r="T1" s="33"/>
@@ -3000,7 +3001,7 @@
         <v>112</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D4" s="14">
         <v>5</v>
@@ -3061,10 +3062,10 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D5" s="14">
         <v>2</v>
@@ -3124,10 +3125,10 @@
     <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="30"/>
       <c r="B6" s="31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D6" s="14">
         <v>2</v>
@@ -3179,10 +3180,10 @@
     <row r="7" spans="1:27" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="48"/>
       <c r="B7" s="24" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D7" s="27">
         <v>1</v>
@@ -3199,7 +3200,7 @@
       <c r="I7" s="27"/>
       <c r="J7" s="27"/>
       <c r="K7" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L7" s="37"/>
       <c r="M7" s="37">
@@ -3225,10 +3226,10 @@
         <v>74</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D8" s="14">
         <v>4</v>
@@ -3247,7 +3248,7 @@
         <v>4</v>
       </c>
       <c r="K8" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L8" s="34"/>
       <c r="M8" s="36">
@@ -3284,7 +3285,7 @@
         <v>113</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D9" s="14">
         <v>2</v>
@@ -3342,7 +3343,7 @@
         <v>114</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D10" s="14">
         <v>5</v>
@@ -3394,7 +3395,7 @@
         <v>115</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D11" s="14">
         <v>2</v>
@@ -3451,10 +3452,10 @@
     </row>
     <row r="12" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D12" s="14">
         <v>9</v>
@@ -3467,7 +3468,7 @@
         <v>10</v>
       </c>
       <c r="K12" s="22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L12" s="34"/>
       <c r="M12" s="36">
@@ -3503,10 +3504,10 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B13" s="23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D13" s="14">
         <v>3</v>
@@ -3565,10 +3566,10 @@
     </row>
     <row r="14" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D14" s="14">
         <v>5</v>
@@ -3581,7 +3582,7 @@
         <v>6</v>
       </c>
       <c r="K14" s="22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L14" s="34"/>
       <c r="M14" s="36">
@@ -3616,10 +3617,10 @@
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B15" s="23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D15" s="14">
         <v>4</v>
@@ -3632,7 +3633,7 @@
         <v>4</v>
       </c>
       <c r="K15" s="22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L15" s="34"/>
       <c r="M15" s="36">
@@ -3673,7 +3674,7 @@
         <v>116</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D16" s="14">
         <v>5</v>
@@ -3732,7 +3733,7 @@
         <v>117</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D17" s="14">
         <v>3</v>
@@ -3776,7 +3777,7 @@
         <v>118</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D18" s="14">
         <v>4</v>
@@ -3825,7 +3826,7 @@
         <v>119</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D19" s="14">
         <v>2</v>
@@ -3883,7 +3884,7 @@
         <v>120</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D20" s="13">
         <v>10</v>
@@ -3940,7 +3941,7 @@
         <v>121</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D21" s="14">
         <v>8</v>
@@ -3988,7 +3989,7 @@
       </c>
       <c r="S21" s="33"/>
       <c r="T21" s="42" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="U21" s="43"/>
       <c r="V21" s="33"/>
@@ -4000,10 +4001,10 @@
     </row>
     <row r="22" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D22" s="14">
         <v>3</v>
@@ -4048,7 +4049,7 @@
         <v>122</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D23" s="14">
         <v>3</v>
@@ -4106,7 +4107,7 @@
         <v>123</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D24" s="14">
         <v>3</v>
@@ -4166,7 +4167,7 @@
         <v>124</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D25" s="14">
         <v>5</v>
@@ -4182,7 +4183,7 @@
         <v>37</v>
       </c>
       <c r="K25" s="57" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="N25" s="34"/>
       <c r="O25" s="34">
@@ -4197,16 +4198,16 @@
       </c>
       <c r="S25" s="33"/>
       <c r="T25" s="46" t="s">
+        <v>170</v>
+      </c>
+      <c r="U25" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="U25" s="4" t="s">
+      <c r="V25" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="V25" s="4" t="s">
+      <c r="W25" s="7" t="s">
         <v>173</v>
-      </c>
-      <c r="W25" s="7" t="s">
-        <v>174</v>
       </c>
       <c r="X25" s="33"/>
       <c r="Y25" s="33"/>
@@ -4218,7 +4219,7 @@
         <v>125</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D26" s="14">
         <v>5</v>
@@ -4231,7 +4232,7 @@
         <v>6</v>
       </c>
       <c r="K26" s="57" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="N26" s="34"/>
       <c r="O26" s="34">
@@ -4249,15 +4250,15 @@
         <v>0</v>
       </c>
       <c r="U26" s="6">
-        <f>SUMIF(R$2:R$75,"&gt;=" &amp; T26,F$2:F$75)</f>
+        <f t="shared" ref="U26:U34" si="2">SUMIF(R$2:R$75,"&gt;=" &amp; T26,F$2:F$75)</f>
         <v>324</v>
       </c>
       <c r="V26" s="6">
-        <f>SUMIF(R$2:R$75,"&gt;=" &amp; T26,E$2:E$75)</f>
+        <f t="shared" ref="V26:V34" si="3">SUMIF(R$2:R$75,"&gt;=" &amp; T26,E$2:E$75)</f>
         <v>16</v>
       </c>
       <c r="W26" s="8">
-        <f t="shared" ref="W26:W34" si="2">($V$17 + $V$15*U26+$V$16*V26)*(1+V$18+V$19)</f>
+        <f t="shared" ref="W26:W34" si="4">($V$17 + $V$15*U26+$V$16*V26)*(1+V$18+V$19)</f>
         <v>31.200000000000003</v>
       </c>
       <c r="X26" s="33"/>
@@ -4273,7 +4274,7 @@
         <v>126</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D27" s="13">
         <v>3</v>
@@ -4294,7 +4295,7 @@
       </c>
       <c r="J27" s="13"/>
       <c r="K27" s="21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L27" s="12"/>
       <c r="M27" s="12"/>
@@ -4315,15 +4316,15 @@
         <v>0.5</v>
       </c>
       <c r="U27" s="6">
-        <f>SUMIF(R$2:R$75,"&gt;=" &amp; T27,F$2:F$75)</f>
+        <f t="shared" si="2"/>
         <v>214</v>
       </c>
       <c r="V27" s="6">
-        <f>SUMIF(R$2:R$75,"&gt;=" &amp; T27,E$2:E$75)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="W27" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>20.930000000000003</v>
       </c>
       <c r="X27" s="33"/>
@@ -4337,7 +4338,7 @@
         <v>127</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D28" s="14">
         <v>2</v>
@@ -4362,7 +4363,7 @@
         <v>15</v>
       </c>
       <c r="K28" s="22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L28" s="2">
         <v>1</v>
@@ -4390,24 +4391,24 @@
         <v>1</v>
       </c>
       <c r="U28" s="6">
-        <f>SUMIF(R$2:R$75,"&gt;=" &amp; T28,F$2:F$75)</f>
+        <f t="shared" si="2"/>
         <v>204</v>
       </c>
       <c r="V28" s="6">
-        <f>SUMIF(R$2:R$75,"&gt;=" &amp; T28,E$2:E$75)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="W28" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>20.28</v>
       </c>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B29" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D29" s="14">
         <v>1</v>
@@ -4423,7 +4424,7 @@
         <v>16</v>
       </c>
       <c r="K29" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L29" s="34"/>
       <c r="M29" s="36">
@@ -4450,15 +4451,15 @@
         <v>1.5</v>
       </c>
       <c r="U29" s="31">
-        <f>SUMIF(R$2:R$75,"&gt;=" &amp; T29,F$2:F$75)</f>
+        <f t="shared" si="2"/>
         <v>194</v>
       </c>
       <c r="V29" s="31">
-        <f>SUMIF(R$2:R$75,"&gt;=" &amp; T29,E$2:E$75)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="W29" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>19.630000000000003</v>
       </c>
       <c r="X29" s="33"/>
@@ -4468,10 +4469,10 @@
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B30" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D30" s="14">
         <v>3</v>
@@ -4496,7 +4497,7 @@
         <v>16</v>
       </c>
       <c r="K30" s="22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L30" s="2">
         <v>1</v>
@@ -4525,15 +4526,15 @@
         <v>2</v>
       </c>
       <c r="U30" s="6">
-        <f>SUMIF(R$2:R$75,"&gt;=" &amp; T30,F$2:F$75)</f>
+        <f t="shared" si="2"/>
         <v>174</v>
       </c>
       <c r="V30" s="6">
-        <f>SUMIF(R$2:R$75,"&gt;=" &amp; T30,E$2:E$75)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="W30" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>18.330000000000002</v>
       </c>
     </row>
@@ -4542,7 +4543,7 @@
         <v>128</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D31" s="14">
         <v>3</v>
@@ -4585,15 +4586,15 @@
         <v>2.5</v>
       </c>
       <c r="U31" s="6">
-        <f>SUMIF(R$2:R$75,"&gt;=" &amp; T31,F$2:F$75)</f>
+        <f t="shared" si="2"/>
         <v>152</v>
       </c>
       <c r="V31" s="6">
-        <f>SUMIF(R$2:R$75,"&gt;=" &amp; T31,E$2:E$75)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="W31" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>16.900000000000002</v>
       </c>
       <c r="X31" s="33"/>
@@ -4606,7 +4607,7 @@
         <v>97</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D32" s="14">
         <v>2</v>
@@ -4654,15 +4655,15 @@
         <v>3</v>
       </c>
       <c r="U32" s="6">
-        <f>SUMIF(R$2:R$75,"&gt;=" &amp; T32,F$2:F$75)</f>
+        <f t="shared" si="2"/>
         <v>148</v>
       </c>
       <c r="V32" s="6">
-        <f>SUMIF(R$2:R$75,"&gt;=" &amp; T32,E$2:E$75)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="W32" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>16.64</v>
       </c>
     </row>
@@ -4672,7 +4673,7 @@
         <v>98</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D33" s="14">
         <v>4</v>
@@ -4691,7 +4692,7 @@
         <v>19</v>
       </c>
       <c r="K33" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L33" s="2"/>
       <c r="M33" s="20">
@@ -4718,15 +4719,15 @@
         <v>3.5</v>
       </c>
       <c r="U33" s="6">
-        <f>SUMIF(R$2:R$75,"&gt;=" &amp; T33,F$2:F$75)</f>
+        <f t="shared" si="2"/>
         <v>130</v>
       </c>
       <c r="V33" s="6">
-        <f>SUMIF(R$2:R$75,"&gt;=" &amp; T33,E$2:E$75)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="W33" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>15.47</v>
       </c>
       <c r="X33"/>
@@ -4739,7 +4740,7 @@
         <v>95</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D34" s="14">
         <v>3</v>
@@ -4755,7 +4756,7 @@
         <v>20</v>
       </c>
       <c r="K34" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M34" s="20">
         <v>1</v>
@@ -4781,15 +4782,15 @@
         <v>4</v>
       </c>
       <c r="U34" s="47">
-        <f>SUMIF(R$2:R$75,"&gt;=" &amp; T34,F$2:F$75)</f>
+        <f t="shared" si="2"/>
         <v>110</v>
       </c>
       <c r="V34" s="47">
-        <f>SUMIF(R$2:R$75,"&gt;=" &amp; T34,E$2:E$75)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="W34" s="9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>14.170000000000002</v>
       </c>
     </row>
@@ -4799,7 +4800,7 @@
         <v>129</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D35" s="14">
         <v>7</v>
@@ -4863,7 +4864,7 @@
         <v>130</v>
       </c>
       <c r="C36" s="26" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D36" s="13">
         <v>2</v>
@@ -4876,7 +4877,7 @@
         <v>2</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H36" s="13">
         <v>23</v>
@@ -4888,7 +4889,7 @@
         <v>22</v>
       </c>
       <c r="K36" s="21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L36" s="12">
         <v>1</v>
@@ -4920,10 +4921,10 @@
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B37" s="23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D37" s="14">
         <v>5</v>
@@ -4977,10 +4978,10 @@
     </row>
     <row r="38" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B38" s="23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D38" s="14">
         <v>4</v>
@@ -4993,7 +4994,7 @@
         <v>4</v>
       </c>
       <c r="K38" s="22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N38" s="34"/>
       <c r="O38" s="33"/>
@@ -5015,7 +5016,7 @@
         <v>131</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D39" s="14">
         <v>6</v>
@@ -5061,10 +5062,10 @@
     </row>
     <row r="40" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B40" s="23" t="s">
-        <v>132</v>
+        <v>218</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D40" s="14">
         <v>5</v>
@@ -5077,7 +5078,7 @@
         <v>6</v>
       </c>
       <c r="G40" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H40" s="14">
         <v>26</v>
@@ -5089,7 +5090,7 @@
         <v>25</v>
       </c>
       <c r="K40" s="22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M40" s="20">
         <v>1</v>
@@ -5121,7 +5122,7 @@
         <v>111</v>
       </c>
       <c r="C41" s="26" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D41" s="13">
         <v>6</v>
@@ -5134,7 +5135,7 @@
         <v>6</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H41" s="13">
         <v>28</v>
@@ -5180,7 +5181,7 @@
         <v>93</v>
       </c>
       <c r="C42" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D42" s="14">
         <v>5</v>
@@ -5193,7 +5194,7 @@
         <v>6</v>
       </c>
       <c r="G42" s="14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H42" s="14">
         <v>29</v>
@@ -5241,10 +5242,10 @@
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B43" s="23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D43" s="14">
         <v>2</v>
@@ -5297,10 +5298,10 @@
     </row>
     <row r="44" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B44" s="23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C44" s="31" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D44" s="14">
         <v>4</v>
@@ -5325,7 +5326,7 @@
         <v>28</v>
       </c>
       <c r="K44" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="N44" s="34"/>
       <c r="O44" s="34"/>
@@ -5347,10 +5348,10 @@
         <v>80</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C45" s="26" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D45" s="13">
         <v>2</v>
@@ -5393,10 +5394,10 @@
     </row>
     <row r="46" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B46" s="23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C46" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D46" s="14">
         <v>3</v>
@@ -5445,10 +5446,10 @@
         <v>81</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C47" s="26" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D47" s="13">
         <v>2</v>
@@ -5500,10 +5501,10 @@
     </row>
     <row r="48" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B48" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C48" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D48" s="14">
         <v>3</v>
@@ -5555,10 +5556,10 @@
     </row>
     <row r="49" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B49" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C49" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D49" s="14">
         <v>3</v>
@@ -5604,10 +5605,10 @@
     <row r="50" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="10"/>
       <c r="B50" s="23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C50" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D50" s="14">
         <v>3</v>
@@ -5656,10 +5657,10 @@
     </row>
     <row r="51" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B51" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C51" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D51" s="14">
         <v>2</v>
@@ -5708,10 +5709,10 @@
     <row r="52" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="10"/>
       <c r="B52" s="23" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C52" s="31" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D52" s="14">
         <v>5</v>
@@ -5766,10 +5767,10 @@
     </row>
     <row r="53" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B53" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C53" s="31" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D53" s="14">
         <v>5</v>
@@ -5817,10 +5818,10 @@
     </row>
     <row r="54" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B54" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C54" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D54" s="14">
         <v>1</v>
@@ -5839,7 +5840,7 @@
         <v>35</v>
       </c>
       <c r="K54" s="22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L54" s="2">
         <v>1</v>
@@ -5874,7 +5875,7 @@
         <v>96</v>
       </c>
       <c r="C55" s="31" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D55" s="14">
         <v>3</v>
@@ -5890,7 +5891,7 @@
         <v>36</v>
       </c>
       <c r="K55" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M55" s="20">
         <v>0.5</v>
@@ -5914,10 +5915,10 @@
     </row>
     <row r="56" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B56" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C56" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D56" s="14">
         <v>5</v>
@@ -5959,10 +5960,10 @@
     </row>
     <row r="57" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B57" s="23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C57" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D57" s="14">
         <v>9</v>
@@ -5996,10 +5997,10 @@
     </row>
     <row r="58" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B58" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C58" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D58" s="14">
         <v>7</v>
@@ -6032,10 +6033,10 @@
     </row>
     <row r="59" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B59" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C59" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D59" s="14">
         <v>5</v>
@@ -6051,7 +6052,7 @@
         <v>38</v>
       </c>
       <c r="K59" s="22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M59" s="20">
         <v>1</v>
@@ -6079,10 +6080,10 @@
         <v>82</v>
       </c>
       <c r="B60" s="26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C60" s="26" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D60" s="13">
         <v>3</v>
@@ -6128,10 +6129,10 @@
     </row>
     <row r="61" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B61" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C61" s="31" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D61" s="14">
         <v>7</v>
@@ -6161,10 +6162,10 @@
     </row>
     <row r="62" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B62" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C62" s="31" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D62" s="14">
         <v>7</v>
@@ -6186,7 +6187,7 @@
         <v>0</v>
       </c>
       <c r="R62" s="77">
-        <f t="shared" ref="R62:R74" si="3">O62+2*P62+Q62</f>
+        <f t="shared" ref="R62:R74" si="5">O62+2*P62+Q62</f>
         <v>0</v>
       </c>
       <c r="S62" s="33"/>
@@ -6198,10 +6199,10 @@
     <row r="63" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A63" s="48"/>
       <c r="B63" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C63" s="24" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D63" s="27">
         <v>10</v>
@@ -6229,7 +6230,7 @@
       </c>
       <c r="Q63" s="90"/>
       <c r="R63" s="79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="S63" s="33"/>
@@ -6241,10 +6242,10 @@
         <v>83</v>
       </c>
       <c r="B64" s="23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C64" s="31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D64" s="14">
         <v>4</v>
@@ -6260,7 +6261,7 @@
         <v>48</v>
       </c>
       <c r="K64" s="22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="N64" s="34"/>
       <c r="O64" s="33"/>
@@ -6268,7 +6269,7 @@
         <v>0</v>
       </c>
       <c r="R64" s="77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="S64" s="33"/>
@@ -6277,10 +6278,10 @@
     <row r="65" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="10"/>
       <c r="B65" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C65" s="31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D65" s="14">
         <v>3</v>
@@ -6308,7 +6309,7 @@
       </c>
       <c r="Q65" s="87"/>
       <c r="R65" s="77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="S65" s="33"/>
@@ -6323,10 +6324,10 @@
     </row>
     <row r="66" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B66" s="23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C66" s="23" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D66" s="14">
         <v>4</v>
@@ -6339,7 +6340,7 @@
         <v>4</v>
       </c>
       <c r="K66" s="22" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="L66" s="87"/>
       <c r="M66" s="89"/>
@@ -6349,7 +6350,7 @@
         <v>1</v>
       </c>
       <c r="R66" s="77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="S66" s="33"/>
@@ -6359,7 +6360,7 @@
         <v>84</v>
       </c>
       <c r="B67" s="26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C67" s="26"/>
       <c r="D67" s="13">
@@ -6396,7 +6397,7 @@
         <v>1</v>
       </c>
       <c r="R67" s="78">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="S67" s="33"/>
@@ -6414,11 +6415,11 @@
         <v>1</v>
       </c>
       <c r="F68" s="14">
-        <f t="shared" ref="F68:F74" si="4">CEILING(D68,T$22+1)</f>
+        <f t="shared" ref="F68:F74" si="6">CEILING(D68,T$22+1)</f>
         <v>2</v>
       </c>
       <c r="K68" s="22" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L68" s="20"/>
       <c r="N68" s="36"/>
@@ -6432,7 +6433,7 @@
         <v>1</v>
       </c>
       <c r="R68" s="77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="S68" s="33"/>
@@ -6442,7 +6443,7 @@
     <row r="69" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="10"/>
       <c r="B69" s="23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C69" s="23"/>
       <c r="D69" s="14">
@@ -6452,7 +6453,7 @@
         <v>3</v>
       </c>
       <c r="F69" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="G69" s="14"/>
@@ -6479,7 +6480,7 @@
         <v>1</v>
       </c>
       <c r="R69" s="77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="S69" s="33"/>
@@ -6494,7 +6495,7 @@
     </row>
     <row r="70" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B70" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D70" s="14">
         <v>1</v>
@@ -6503,7 +6504,7 @@
         <v>0</v>
       </c>
       <c r="F70" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="K70" s="22" t="s">
@@ -6525,7 +6526,7 @@
         <v>1</v>
       </c>
       <c r="R70" s="77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="S70" s="33"/>
@@ -6537,7 +6538,7 @@
     <row r="71" spans="1:27" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="10"/>
       <c r="B71" s="23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C71" s="23"/>
       <c r="D71" s="14">
@@ -6547,7 +6548,7 @@
         <v>1</v>
       </c>
       <c r="F71" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="G71" s="14"/>
@@ -6559,7 +6560,7 @@
       <c r="M71" s="20"/>
       <c r="N71" s="34"/>
       <c r="R71" s="77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="T71" s="3"/>
@@ -6573,7 +6574,7 @@
     </row>
     <row r="72" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B72" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D72" s="14">
         <v>1</v>
@@ -6582,7 +6583,7 @@
         <v>0</v>
       </c>
       <c r="F72" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="K72" s="22"/>
@@ -6591,14 +6592,14 @@
       <c r="P72" s="33"/>
       <c r="Q72" s="33"/>
       <c r="R72" s="77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="S72" s="33"/>
     </row>
     <row r="73" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B73" s="23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D73" s="14">
         <v>4</v>
@@ -6607,7 +6608,7 @@
         <v>0</v>
       </c>
       <c r="F73" s="14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="K73" s="22"/>
@@ -6618,7 +6619,7 @@
       <c r="P73" s="33"/>
       <c r="Q73" s="33"/>
       <c r="R73" s="77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="S73" s="33"/>
@@ -6629,7 +6630,7 @@
     <row r="74" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="10"/>
       <c r="B74" s="24" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C74" s="24"/>
       <c r="D74" s="27">
@@ -6639,7 +6640,7 @@
         <v>0</v>
       </c>
       <c r="F74" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="G74" s="27"/>
@@ -6647,7 +6648,7 @@
       <c r="I74" s="27"/>
       <c r="J74" s="27"/>
       <c r="K74" s="29" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L74" s="28"/>
       <c r="M74" s="28">
@@ -6664,7 +6665,7 @@
         <v>1</v>
       </c>
       <c r="R74" s="79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="S74" s="15"/>
@@ -6683,7 +6684,7 @@
     </row>
     <row r="76" spans="1:27" x14ac:dyDescent="0.3">
       <c r="K76" s="64" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L76" s="65">
         <f t="array" ref="L76">SUM($F2:$F74*(L2:L74&gt;=0.9)*($R2:$R74&gt;=$T$12))</f>
@@ -6717,7 +6718,7 @@
     </row>
     <row r="77" spans="1:27" x14ac:dyDescent="0.3">
       <c r="K77" s="67" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L77" s="68">
         <f t="array" ref="L77">SUM($F2:$F74*L2:L74*($R2:$R74&gt;=$T$12))</f>
@@ -6757,7 +6758,7 @@
       <c r="I78" s="14"/>
       <c r="J78" s="14"/>
       <c r="K78" s="67" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L78" s="68">
         <f t="array" ref="L78">SUM($F$2:$F$74*(L$2:L$74&gt;=0.1)*($R$2:$R$74&gt;=$T$12))</f>
@@ -6796,59 +6797,59 @@
     </row>
     <row r="79" spans="1:27" x14ac:dyDescent="0.3">
       <c r="K79" s="67" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L79" s="68">
-        <f t="shared" ref="L79:Q79" si="5">LOOKUP($T$12,$T26:$T34,$U26:$U34)</f>
+        <f t="shared" ref="L79:Q79" si="7">LOOKUP($T$12,$T26:$T34,$U26:$U34)</f>
         <v>194</v>
       </c>
       <c r="M79" s="68">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>194</v>
       </c>
       <c r="N79" s="68">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>194</v>
       </c>
       <c r="O79" s="68">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>194</v>
       </c>
       <c r="P79" s="68">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>194</v>
       </c>
       <c r="Q79" s="69">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>194</v>
       </c>
     </row>
     <row r="80" spans="1:27" x14ac:dyDescent="0.3">
       <c r="K80" s="67" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L80" s="70">
-        <f t="shared" ref="L80:N80" si="6">L77/L79</f>
+        <f t="shared" ref="L80:N80" si="8">L77/L79</f>
         <v>0.50515463917525771</v>
       </c>
       <c r="M80" s="70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.79072164948453616</v>
       </c>
       <c r="N80" s="70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.80927835051546393</v>
       </c>
       <c r="O80" s="70">
-        <f t="shared" ref="O80:P80" si="7">O77/O79</f>
+        <f t="shared" ref="O80:P80" si="9">O77/O79</f>
         <v>0.83711340206185569</v>
       </c>
       <c r="P80" s="70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.87010309278350517</v>
       </c>
       <c r="Q80" s="71">
-        <f t="shared" ref="Q80" si="8">Q77/Q79</f>
+        <f t="shared" ref="Q80" si="10">Q77/Q79</f>
         <v>0.81597938144329907</v>
       </c>
       <c r="U80" s="33"/>

</xml_diff>